<commit_message>
Domergowanie do dokumentacji koncowej komunikacji
</commit_message>
<xml_diff>
--- a/PodsumowaniaSpotkan/zadania.xlsx
+++ b/PodsumowaniaSpotkan/zadania.xlsx
@@ -506,7 +506,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,16 +516,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B7:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="40.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53" customWidth="1"/>
     <col min="8" max="8" width="50.28515625" customWidth="1"/>
     <col min="9" max="9" width="30.5703125" customWidth="1"/>
     <col min="10" max="10" width="32.5703125" customWidth="1"/>

</xml_diff>